<commit_message>
add some test data
</commit_message>
<xml_diff>
--- a/resources/data_sheets/user_credentials.xlsx
+++ b/resources/data_sheets/user_credentials.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
@@ -33,15 +33,6 @@
   </si>
   <si>
     <t>admin</t>
-  </si>
-  <si>
-    <t>tom</t>
-  </si>
-  <si>
-    <t>ron</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> or 1=1 -- -</t>
   </si>
   <si>
     <t>admin'</t>
@@ -455,10 +446,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A3" sqref="A3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,43 +475,19 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
+      <c r="A4" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>1212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>